<commit_message>
added one json for time bucket analysis
</commit_message>
<xml_diff>
--- a/statistics/HistoricalDistanceData/historical_distance/Q10681317-en.xlsx
+++ b/statistics/HistoricalDistanceData/historical_distance/Q10681317-en.xlsx
@@ -31,37 +31,37 @@
     <t>uri</t>
   </si>
   <si>
+    <t>Tornado History Project: March 13, 1993</t>
+  </si>
+  <si>
     <t>Where were you during the Blizzard of '93? AL.com wants your pictures, memories</t>
   </si>
   <si>
-    <t>Tornado History Project: March 13, 1993</t>
-  </si>
-  <si>
     <t>Birmingham Cold Weather Facts</t>
   </si>
   <si>
+    <t>1993-03-13T00:00:00UTC</t>
+  </si>
+  <si>
     <t>2013-03-07T13:00:00UTC</t>
   </si>
   <si>
-    <t>1993-03-13T00:00:00UTC</t>
-  </si>
-  <si>
     <t>1-01-01T00:00:00UTC</t>
   </si>
   <si>
     <t>unknown</t>
   </si>
   <si>
+    <t>day_2_to_30</t>
+  </si>
+  <si>
     <t>day_31_beyond</t>
   </si>
   <si>
-    <t>day_2_to_30</t>
+    <t>http://www.tornadohistoryproject.com/tornado/1993/3/13/table</t>
   </si>
   <si>
     <t>http://blog.al.com/spotnews/2013/03/where_were_you_during_the_bliz.html</t>
-  </si>
-  <si>
-    <t>http://www.tornadohistoryproject.com/tornado/1993/3/13/table</t>
   </si>
   <si>
     <t>http://www.srh.noaa.gov/bmx/?n=climo_winter2006bhm</t>
@@ -466,7 +466,7 @@
         <v>8</v>
       </c>
       <c r="C2">
-        <v>7311</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -483,7 +483,7 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>12</v>
+        <v>7311</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>

</xml_diff>